<commit_message>
working on top 10 lists page - parsing JSON
</commit_message>
<xml_diff>
--- a/support/most_affordable_sd.xlsx
+++ b/support/most_affordable_sd.xlsx
@@ -18,39 +18,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Strret Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Extraction</t>
-  </si>
-  <si>
-    <t>Root Canal</t>
-  </si>
-  <si>
     <t>San Diego Smile Dentistry</t>
   </si>
   <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
     <t>SD Smile</t>
   </si>
   <si>
@@ -63,9 +33,6 @@
     <t>CA</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>Great Smile Dental</t>
   </si>
   <si>
@@ -75,9 +42,6 @@
     <t>5210 Balboa Ave</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
     <t>Kearny Mesa</t>
   </si>
   <si>
@@ -168,15 +132,6 @@
     <t>7625 Mesa College Dr</t>
   </si>
   <si>
-    <t>Composite Filling - 1 surface</t>
-  </si>
-  <si>
-    <t>Adult Cleaning</t>
-  </si>
-  <si>
-    <t>Porcelain Crown</t>
-  </si>
-  <si>
     <t>Average SD from BracesInfo.com</t>
   </si>
   <si>
@@ -201,9 +156,6 @@
     <t>voicemail</t>
   </si>
   <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Tom (after 9:30 AM) - called back, was given email address sdsmiledentist@gmail.com</t>
   </si>
   <si>
@@ -256,6 +208,54 @@
   </si>
   <si>
     <t>Hillcrest</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>abbreviation</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>adult_cleaning</t>
+  </si>
+  <si>
+    <t>composite_filling</t>
+  </si>
+  <si>
+    <t>extraction</t>
+  </si>
+  <si>
+    <t>root_canal</t>
+  </si>
+  <si>
+    <t>porcelain_crown</t>
+  </si>
+  <si>
+    <t>website</t>
   </si>
 </sst>
 </file>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,75 +686,75 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G2" s="5">
         <v>92111</v>
@@ -769,30 +769,30 @@
         <v>-117.15791299999999</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G3" s="5">
         <v>92117</v>
@@ -812,30 +812,30 @@
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="13" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="Q3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G4" s="5">
         <v>92110</v>
@@ -857,30 +857,30 @@
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
       <c r="P4" s="13" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="Q4" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G5" s="5">
         <v>92117</v>
@@ -895,30 +895,30 @@
         <v>-117.210185</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="Q5" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G6" s="5">
         <v>92122</v>
@@ -948,30 +948,30 @@
         <v>1350</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="Q6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G7" s="5">
         <v>92104</v>
@@ -991,30 +991,30 @@
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
       <c r="P7" s="13" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="Q7" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G8" s="5">
         <v>91942</v>
@@ -1036,30 +1036,30 @@
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
       <c r="P8" s="13" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="Q8" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G9" s="5">
         <v>92120</v>
@@ -1079,30 +1079,30 @@
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
       <c r="P9" s="13" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="Q9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G10" s="5">
         <v>92111</v>
@@ -1122,30 +1122,30 @@
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="Q10" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G11" s="5">
         <v>92111</v>
@@ -1165,15 +1165,15 @@
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
       <c r="P11" s="13" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="Q11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="K13" s="9">
         <v>73</v>
@@ -1198,22 +1198,22 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G16" s="5">
         <v>92103</v>
@@ -1243,7 +1243,7 @@
         <v>1392</v>
       </c>
       <c r="P16" s="13" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="14:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working on graphs and don't want to lose what I have
</commit_message>
<xml_diff>
--- a/support/most_affordable_sd.xlsx
+++ b/support/most_affordable_sd.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>San Diego Smile Dentistry</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>website</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>fake_data</t>
   </si>
 </sst>
 </file>
@@ -268,7 +274,7 @@
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +301,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,7 +339,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,6 +366,11 @@
     <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -657,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,10 +698,11 @@
     <col min="14" max="14" width="14.28515625" style="9" customWidth="1"/>
     <col min="15" max="15" width="10.42578125" style="9" customWidth="1"/>
     <col min="16" max="16" width="67.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="79" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="9" customWidth="1"/>
+    <col min="18" max="18" width="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -733,11 +751,14 @@
       <c r="P1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -768,14 +789,32 @@
       <c r="J2">
         <v>-117.15791299999999</v>
       </c>
+      <c r="K2" s="11">
+        <v>105</v>
+      </c>
+      <c r="L2" s="11">
+        <v>140</v>
+      </c>
+      <c r="M2" s="11">
+        <v>110</v>
+      </c>
+      <c r="N2" s="11">
+        <v>725</v>
+      </c>
+      <c r="O2" s="11">
+        <v>850</v>
+      </c>
       <c r="P2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="R2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -806,19 +845,32 @@
       <c r="J3">
         <v>-117.18396799999999</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="K3" s="11">
+        <v>95</v>
+      </c>
+      <c r="L3" s="11">
+        <v>120</v>
+      </c>
+      <c r="M3" s="11">
+        <v>110</v>
+      </c>
+      <c r="N3" s="11">
+        <v>765</v>
+      </c>
+      <c r="O3" s="11">
+        <v>1105</v>
+      </c>
       <c r="P3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -852,18 +904,29 @@
       <c r="K4" s="9">
         <v>100</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
+      <c r="L4" s="11">
+        <v>120</v>
+      </c>
+      <c r="M4" s="11">
+        <v>125</v>
+      </c>
+      <c r="N4" s="11">
+        <v>785</v>
+      </c>
+      <c r="O4" s="11">
+        <v>950</v>
+      </c>
       <c r="P4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -894,14 +957,32 @@
       <c r="J5">
         <v>-117.210185</v>
       </c>
+      <c r="K5" s="11">
+        <v>110</v>
+      </c>
+      <c r="L5" s="11">
+        <v>135</v>
+      </c>
+      <c r="M5" s="11">
+        <v>130</v>
+      </c>
+      <c r="N5" s="11">
+        <v>780</v>
+      </c>
+      <c r="O5" s="11">
+        <v>1100</v>
+      </c>
       <c r="P5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -950,11 +1031,12 @@
       <c r="P6" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="15"/>
+      <c r="R6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -985,19 +1067,32 @@
       <c r="J7">
         <v>-117.130512</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
+      <c r="K7" s="11">
+        <v>120</v>
+      </c>
+      <c r="L7" s="11">
+        <v>180</v>
+      </c>
+      <c r="M7" s="11">
+        <v>180</v>
+      </c>
+      <c r="N7" s="11">
+        <v>810</v>
+      </c>
+      <c r="O7" s="11">
+        <v>1150</v>
+      </c>
       <c r="P7" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="R7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1031,18 +1126,29 @@
       <c r="K8" s="9">
         <v>100</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="L8" s="11">
+        <v>160</v>
+      </c>
+      <c r="M8" s="11">
+        <v>170</v>
+      </c>
+      <c r="N8" s="11">
+        <v>795</v>
+      </c>
+      <c r="O8" s="11">
+        <v>1010</v>
+      </c>
       <c r="P8" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="R8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1073,19 +1179,32 @@
       <c r="J9">
         <v>-117.098264</v>
       </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="K9" s="11">
+        <v>107</v>
+      </c>
+      <c r="L9" s="11">
+        <v>175</v>
+      </c>
+      <c r="M9" s="11">
+        <v>155</v>
+      </c>
+      <c r="N9" s="11">
+        <v>805</v>
+      </c>
+      <c r="O9" s="11">
+        <v>965</v>
+      </c>
       <c r="P9" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="R9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1116,19 +1235,32 @@
       <c r="J10">
         <v>-117.160985</v>
       </c>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
+      <c r="K10" s="11">
+        <v>110</v>
+      </c>
+      <c r="L10" s="11">
+        <v>150</v>
+      </c>
+      <c r="M10" s="11">
+        <v>160</v>
+      </c>
+      <c r="N10" s="11">
+        <v>810</v>
+      </c>
+      <c r="O10" s="11">
+        <v>890</v>
+      </c>
       <c r="P10" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="R10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1159,19 +1291,35 @@
       <c r="J11">
         <v>-117.157321</v>
       </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
+      <c r="K11" s="11">
+        <v>100</v>
+      </c>
+      <c r="L11" s="11">
+        <v>130</v>
+      </c>
+      <c r="M11" s="11">
+        <v>150</v>
+      </c>
+      <c r="N11" s="11">
+        <v>750</v>
+      </c>
+      <c r="O11" s="11">
+        <v>1010</v>
+      </c>
       <c r="P11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q12" s="18"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1190,13 +1338,18 @@
       <c r="O13" s="9">
         <v>751</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q13" s="18"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N14" s="9">
         <v>802</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q14" s="18"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q15" s="18"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1245,6 +1398,7 @@
       <c r="P16" s="13" t="s">
         <v>59</v>
       </c>
+      <c r="Q16" s="15"/>
     </row>
     <row r="17" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N17" s="9">

</xml_diff>